<commit_message>
implementation grading sheet hw6 claimed
</commit_message>
<xml_diff>
--- a/implementation-grading-sheet-SADGE_GOOMBAS.xlsx
+++ b/implementation-grading-sheet-SADGE_GOOMBAS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin\home\stoller\courses\software-engg-2021\pub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\tseyt\documents\_vscode\CSE416-Masters_Student_Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58F80FD-E5CA-4BBF-8F10-4177112105BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A907FB02-EE36-4E25-B80B-7034A893C8F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15690" yWindow="375" windowWidth="18135" windowHeight="20415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -700,7 +700,7 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -808,7 +808,9 @@
       <c r="B6" s="16">
         <v>12</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="16">
+        <v>12</v>
+      </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -858,7 +860,9 @@
       <c r="B10" s="4">
         <v>4</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4">
+        <v>4</v>
+      </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -872,7 +876,9 @@
       <c r="B11" s="4">
         <v>4</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="4">
+        <v>4</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -886,7 +892,9 @@
       <c r="B12" s="4">
         <v>2</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4">
+        <v>2</v>
+      </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -900,7 +908,9 @@
       <c r="B13" s="4">
         <v>4</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="4">
+        <v>4</v>
+      </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -914,7 +924,9 @@
       <c r="B14" s="4">
         <v>4</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="4">
+        <v>4</v>
+      </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -928,7 +940,9 @@
       <c r="B15" s="4">
         <v>5</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="4">
+        <v>5</v>
+      </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -1250,31 +1264,31 @@
         <v>0</v>
       </c>
       <c r="B42" s="4">
-        <f>SUM(B1:B41)</f>
+        <f t="shared" ref="B42:H42" si="0">SUM(B1:B41)</f>
         <v>100</v>
       </c>
       <c r="C42" s="4">
-        <f>SUM(C1:C41)</f>
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D42" s="4">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D42" s="4">
-        <f>SUM(D1:D41)</f>
+      <c r="E42" s="4">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E42" s="4">
-        <f>SUM(E1:E41)</f>
+      <c r="F42" s="4">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F42" s="4">
-        <f>SUM(F1:F41)</f>
+      <c r="G42" s="4">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G42" s="4">
-        <f>SUM(G1:G41)</f>
-        <v>0</v>
-      </c>
       <c r="H42" s="4">
-        <f>SUM(H1:H41)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
claimed points for hw7
</commit_message>
<xml_diff>
--- a/implementation-grading-sheet-SADGE_GOOMBAS.xlsx
+++ b/implementation-grading-sheet-SADGE_GOOMBAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\tseyt\documents\_vscode\CSE416-Masters_Student_Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED7361A-9B8C-44CB-854A-40C43F44E55B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD52D437-5562-4E8B-950D-D507B68FEB06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="1710" windowWidth="23760" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -700,7 +700,7 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -958,7 +958,9 @@
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="E16" s="4">
+        <v>12</v>
+      </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -972,7 +974,9 @@
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4">
+        <v>13</v>
+      </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
@@ -986,7 +990,9 @@
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="E18" s="4">
+        <v>12</v>
+      </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
@@ -1000,7 +1006,9 @@
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="E19" s="4">
+        <v>5</v>
+      </c>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
@@ -1036,7 +1044,9 @@
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="E22" s="4">
+        <v>3</v>
+      </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
@@ -1050,7 +1060,9 @@
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+      <c r="E23" s="4">
+        <v>2</v>
+      </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -1277,7 +1289,7 @@
       </c>
       <c r="E42" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="F42" s="4">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
feat(auth): login UI and set studentID in vuex store
</commit_message>
<xml_diff>
--- a/implementation-grading-sheet-SADGE_GOOMBAS.xlsx
+++ b/implementation-grading-sheet-SADGE_GOOMBAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\tseyt\documents\_vscode\CSE416-Masters_Student_Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD52D437-5562-4E8B-950D-D507B68FEB06}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E8A033-9032-4CCA-BFE5-D993CFD656DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1710" windowWidth="23760" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -699,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -811,7 +811,9 @@
       <c r="C6" s="16">
         <v>12</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="16">
+        <v>12</v>
+      </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -863,7 +865,9 @@
       <c r="C10" s="4">
         <v>4</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4">
+        <v>4</v>
+      </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -879,7 +883,9 @@
       <c r="C11" s="4">
         <v>4</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="4">
+        <v>4</v>
+      </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -895,7 +901,9 @@
       <c r="C12" s="4">
         <v>2</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="4">
+        <v>2</v>
+      </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
@@ -911,7 +919,9 @@
       <c r="C13" s="4">
         <v>4</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="4">
+        <v>4</v>
+      </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -927,7 +937,9 @@
       <c r="C14" s="4">
         <v>4</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="4">
+        <v>4</v>
+      </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -943,7 +955,9 @@
       <c r="C15" s="4">
         <v>5</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="4">
+        <v>5</v>
+      </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -1098,7 +1112,9 @@
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
+      <c r="E26" s="4">
+        <v>4</v>
+      </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
@@ -1124,7 +1140,9 @@
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
+      <c r="E28" s="4">
+        <v>5</v>
+      </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -1138,7 +1156,9 @@
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
+      <c r="E29" s="4">
+        <v>2</v>
+      </c>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
@@ -1152,7 +1172,9 @@
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
+      <c r="E30" s="4">
+        <v>2</v>
+      </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
@@ -1285,11 +1307,11 @@
       </c>
       <c r="D42" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="E42" s="4">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="F42" s="4">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
fix(view-edit): setting studentID state in v-e-GPD from route
</commit_message>
<xml_diff>
--- a/implementation-grading-sheet-SADGE_GOOMBAS.xlsx
+++ b/implementation-grading-sheet-SADGE_GOOMBAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\tseyt\documents\_vscode\CSE416-Masters_Student_Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E8A033-9032-4CCA-BFE5-D993CFD656DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380C82EA-BC03-48D7-9CAA-7213927A6602}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -699,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
feat(docs): added concurrency section to readme, and updated impl status
</commit_message>
<xml_diff>
--- a/implementation-grading-sheet-SADGE_GOOMBAS.xlsx
+++ b/implementation-grading-sheet-SADGE_GOOMBAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\tseyt\documents\_vscode\CSE416-Masters_Student_Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380C82EA-BC03-48D7-9CAA-7213927A6602}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51888317-2D52-4C89-9DC5-99ECCE913C89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="1710" windowWidth="23760" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -699,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>